<commit_message>
update: improvements in app
</commit_message>
<xml_diff>
--- a/MCAP31122023.xlsx
+++ b/MCAP31122023.xlsx
@@ -13660,7 +13660,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -13670,6 +13670,12 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -13747,10 +13753,10 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -14096,7 +14102,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -14110,7 +14116,7 @@
         <v>174889554.787729</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -14124,7 +14130,7 @@
         <v>137248531.907812</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -14138,7 +14144,7 @@
         <v>129740453.99988699</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -14152,7 +14158,7 @@
         <v>69902440.891932</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -14166,7 +14172,7 @@
         <v>64037070.702681</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -14180,7 +14186,7 @@
         <v>62591936.424049005</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -14194,7 +14200,7 @@
         <v>58028012.499392</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -14208,7 +14214,7 @@
         <v>57649787.673312</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -14222,7 +14228,7 @@
         <v>57300470.922247</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -14236,7 +14242,7 @@
         <v>52655605.860825</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -14250,7 +14256,7 @@
         <v>48466573.5869</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -14264,7 +14270,7 @@
         <v>45287186.0248675</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="4">
         <v>13</v>
       </c>

</xml_diff>